<commit_message>
update tableau de tache
</commit_message>
<xml_diff>
--- a/Docs/Tableau Répartition des tâches .xlsx
+++ b/Docs/Tableau Répartition des tâches .xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\enzor\OneDrive\Documents\Projet_Red\Crayston-Viollet-Rossi-red\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C5FFAA9E-A1D8-48C6-A1CE-937DB515A711}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF9E3A8B-87B5-4415-ADD5-6A047FA858F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13695" xr2:uid="{D993ECAD-6A51-4057-BDCD-6F7376C6584B}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>Liste
 des Tâches</t>
@@ -68,6 +68,9 @@
   </si>
   <si>
     <t>Gestion du git arragement du programme et package</t>
+  </si>
+  <si>
+    <t>Creation et gestion forgeron</t>
   </si>
 </sst>
 </file>
@@ -422,10 +425,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89C5E5FB-552F-4A9B-9402-9C9D6C0A9CC9}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -433,7 +436,7 @@
     <col min="5" max="5" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" ht="57" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -449,8 +452,11 @@
       <c r="E1" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="F1" s="1" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -464,6 +470,9 @@
         <v>8</v>
       </c>
       <c r="E2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add menu inventaire et ajout equipement
</commit_message>
<xml_diff>
--- a/Docs/Tableau Répartition des tâches .xlsx
+++ b/Docs/Tableau Répartition des tâches .xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\enzor\OneDrive\Documents\Projet_Red\Crayston-Viollet-Rossi-red\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF9E3A8B-87B5-4415-ADD5-6A047FA858F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BE0F534-812E-4C9E-B875-5A881785B72F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13695" xr2:uid="{D993ECAD-6A51-4057-BDCD-6F7376C6584B}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
   <si>
     <t>Liste
 des Tâches</t>
@@ -71,6 +71,12 @@
   </si>
   <si>
     <t>Creation et gestion forgeron</t>
+  </si>
+  <si>
+    <t>Creation monstre et equipement</t>
+  </si>
+  <si>
+    <t>Gestion equipement</t>
   </si>
 </sst>
 </file>
@@ -425,10 +431,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89C5E5FB-552F-4A9B-9402-9C9D6C0A9CC9}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -436,7 +442,7 @@
     <col min="5" max="5" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="57" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8" ht="57" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -455,8 +461,14 @@
       <c r="F1" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="G1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -473,6 +485,12 @@
         <v>6</v>
       </c>
       <c r="F2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add armes and change classe
</commit_message>
<xml_diff>
--- a/Docs/Tableau Répartition des tâches .xlsx
+++ b/Docs/Tableau Répartition des tâches .xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\enzor\OneDrive\Documents\Projet_Red\Crayston-Viollet-Rossi-red\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC271B8D-402B-404A-BBB3-D569863B9D11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E2D3CD7-9F2A-404D-8CD9-5805C488CF76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13695" xr2:uid="{D993ECAD-6A51-4057-BDCD-6F7376C6584B}"/>
+    <workbookView xWindow="5047" yWindow="368" windowWidth="16200" windowHeight="9900" xr2:uid="{D993ECAD-6A51-4057-BDCD-6F7376C6584B}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="24">
   <si>
     <t>Liste
 des Tâches</t>
@@ -48,56 +48,68 @@
   </si>
   <si>
     <t>Création et 
-gestion du menu</t>
+gestion de l'argent</t>
+  </si>
+  <si>
+    <t>Yoan</t>
+  </si>
+  <si>
+    <t>Enzo</t>
+  </si>
+  <si>
+    <t>Enzo &amp; Yoan</t>
+  </si>
+  <si>
+    <t>Matt</t>
+  </si>
+  <si>
+    <t>Gestion du git arragement du programme et package</t>
+  </si>
+  <si>
+    <t>Creation et gestion forgeron</t>
+  </si>
+  <si>
+    <t>Creation monstre et equipement</t>
+  </si>
+  <si>
+    <t>Gestion equipement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Optimisation et arragement du code </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gestion et création marchand </t>
+  </si>
+  <si>
+    <t>Gestion Invertaire</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Système potion </t>
+  </si>
+  <si>
+    <t>Matt &amp; Yoan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gestion combat </t>
+  </si>
+  <si>
+    <t>Gestion Experience</t>
+  </si>
+  <si>
+    <t>Gestion Skill et mana</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yoan </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Matt </t>
   </si>
   <si>
     <t>Création et 
-gestion de l'argent</t>
-  </si>
-  <si>
-    <t>Yoan</t>
-  </si>
-  <si>
-    <t>Enzo</t>
-  </si>
-  <si>
-    <t>Enzo &amp; Yoan</t>
-  </si>
-  <si>
-    <t>Matt</t>
-  </si>
-  <si>
-    <t>Gestion du git arragement du programme et package</t>
-  </si>
-  <si>
-    <t>Creation et gestion forgeron</t>
-  </si>
-  <si>
-    <t>Creation monstre et equipement</t>
-  </si>
-  <si>
-    <t>Gestion equipement</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Optimisation et arragement du code </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gestion et création marchand </t>
-  </si>
-  <si>
-    <t>Gestion Invertaire</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Système potion </t>
-  </si>
-  <si>
-    <t>Gestion Skill</t>
-  </si>
-  <si>
-    <t>Matt &amp; Yoan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gestion combat </t>
+gestion des menu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gestion erreur </t>
   </si>
 </sst>
 </file>
@@ -452,10 +464,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89C5E5FB-552F-4A9B-9402-9C9D6C0A9CC9}">
-  <dimension ref="A1:N2"/>
+  <dimension ref="A1:P2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N3" sqref="N3"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -464,7 +476,7 @@
     <col min="9" max="9" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="57" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:16" ht="57" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -472,84 +484,93 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="E1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="M1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="N1" s="1" t="s">
-        <v>19</v>
+      <c r="O1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:16" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
+      <c r="F2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" t="s">
+        <v>5</v>
+      </c>
+      <c r="J2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="K2" t="s">
+        <v>21</v>
+      </c>
+      <c r="L2" t="s">
+        <v>4</v>
+      </c>
+      <c r="M2" t="s">
+        <v>20</v>
+      </c>
+      <c r="N2" t="s">
+        <v>16</v>
+      </c>
+      <c r="O2" t="s">
         <v>5</v>
-      </c>
-      <c r="H2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I2" t="s">
-        <v>6</v>
-      </c>
-      <c r="J2" t="s">
-        <v>8</v>
-      </c>
-      <c r="K2" t="s">
-        <v>18</v>
-      </c>
-      <c r="L2" t="s">
-        <v>5</v>
-      </c>
-      <c r="M2" t="s">
-        <v>8</v>
-      </c>
-      <c r="N2" t="s">
-        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Correct forge and add exit
</commit_message>
<xml_diff>
--- a/Docs/Tableau Répartition des tâches .xlsx
+++ b/Docs/Tableau Répartition des tâches .xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\enzor\OneDrive\Documents\Projet_Red\Crayston-Viollet-Rossi-red\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E2D3CD7-9F2A-404D-8CD9-5805C488CF76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A21D614D-A74E-4580-8460-BE8EBAF0CAC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5047" yWindow="368" windowWidth="16200" windowHeight="9900" xr2:uid="{D993ECAD-6A51-4057-BDCD-6F7376C6584B}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="24">
   <si>
     <t>Liste
 des Tâches</t>
@@ -467,7 +467,7 @@
   <dimension ref="A1:P2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="P2" sqref="P2"/>
+      <selection activeCell="P3" sqref="P3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -572,6 +572,9 @@
       <c r="O2" t="s">
         <v>5</v>
       </c>
+      <c r="P2" t="s">
+        <v>4</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>